<commit_message>
C++/Python Solution for DSA problems
</commit_message>
<xml_diff>
--- a/DSA by Shradha Ma'am.xlsx
+++ b/DSA by Shradha Ma'am.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Data Analyst Course\Coding Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Data Analyst Course\Coding-Practice-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783A9D5D-0A73-4103-A1C4-182B643648B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C78686B-46FA-4CD2-BF98-45EA97B2A446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,16 +24,16 @@
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{037F9168-0D33-45AB-8FA5-B5F97D423138}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{FBEC9E1E-B245-48FE-BAF6-DAD243A465DA}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{EC5A45E8-31C4-490F-BC89-C0A47B108A6A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{F4DD247F-6B0D-42AF-8847-65EF4ED94328}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{EC5A45E8-31C4-490F-BC89-C0A47B108A6A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{FBEC9E1E-B245-48FE-BAF6-DAD243A465DA}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{037F9168-0D33-45AB-8FA5-B5F97D423138}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="703">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2742,8 +2742,8 @@
   </sheetPr>
   <dimension ref="A1:Z919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3185,8 +3185,12 @@
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>702</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -4215,8 +4219,12 @@
         <v>73</v>
       </c>
       <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="E44" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>702</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -30638,21 +30646,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{037F9168-0D33-45AB-8FA5-B5F97D423138}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{EC5A45E8-31C4-490F-BC89-C0A47B108A6A}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{6BE74607-F88A-4072-8DB5-993327AE766E}"/>
+      <autoFilter ref="A11:C37" xr:uid="{9A16F6ED-FE87-4D0B-BC1B-EE3DC5A9CA39}"/>
+    </customSheetView>
+    <customSheetView guid="{FBEC9E1E-B245-48FE-BAF6-DAD243A465DA}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{AAEA8C19-8CD1-4823-BF2E-70F8D89FA1C0}"/>
     </customSheetView>
     <customSheetView guid="{F4DD247F-6B0D-42AF-8847-65EF4ED94328}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{1887BA1E-8EA2-4E96-8FF5-18375328FA1B}"/>
+      <autoFilter ref="A11:D37" xr:uid="{5FF6B4B6-3C79-4483-8C7A-0A36497B35C8}"/>
     </customSheetView>
-    <customSheetView guid="{FBEC9E1E-B245-48FE-BAF6-DAD243A465DA}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{037F9168-0D33-45AB-8FA5-B5F97D423138}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{04215499-E767-44BB-88F0-E14B30127B7D}"/>
-    </customSheetView>
-    <customSheetView guid="{EC5A45E8-31C4-490F-BC89-C0A47B108A6A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{3E5D3AAC-BBBE-43EF-8BB9-8A640C0B026D}"/>
+      <autoFilter ref="A293:C332" xr:uid="{11913A38-0CCC-44D4-9239-524373586A7F}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">

</xml_diff>